<commit_message>
analysis of more datasets
</commit_message>
<xml_diff>
--- a/phaseshift/phaseshift_summary.xlsx
+++ b/phaseshift/phaseshift_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/phaseshift/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD0C6356-A5A2-2348-9876-02F6C794A9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDD1226-981F-A548-965B-544FEB6B3849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1360" windowWidth="28040" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phaseshift_metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>filename</t>
   </si>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>Bcal_run</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>2024-04-12_K_UHfit.dat</t>
+  </si>
+  <si>
+    <t>2024-04-12_L_UHfit.dat</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>2024-03-05_E</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>2024-04-15_I_UHfit.dat</t>
   </si>
 </sst>
 </file>
@@ -897,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,6 +984,93 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45394</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>1.8</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>202.14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45394</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>0.9</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>202.14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45397</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>0.9</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>202.14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
April 26 data analysis
</commit_message>
<xml_diff>
--- a/phaseshift/phaseshift_summary.xlsx
+++ b/phaseshift/phaseshift_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/phaseshift/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDD1226-981F-A548-965B-544FEB6B3849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FD4EB8-8A1A-3D42-AECC-8558959EDA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phaseshift_metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>filename</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>2024-04-15_I_UHfit.dat</t>
+  </si>
+  <si>
+    <t>2024-04-26_D_e.dat</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>2023-11-13_E</t>
   </si>
 </sst>
 </file>
@@ -918,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,6 +1080,35 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45408</v>
+      </c>
+      <c r="E6">
+        <v>2.5</v>
+      </c>
+      <c r="F6">
+        <v>1.8</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>202.1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
analysis as of May 12
a bunch of data files and some analysis files for 2 kHz HFT and 5 kHz dimer loss.
2 kHz HFT analysis is WIP, currently testing out chi2-of-free-phase-fit analysis.
5 kHz dimer is separated into Apr 30, May2, and May 10 analysis. There are some specifics but they share a lot of code. May2 is the most "standard" one.
</commit_message>
<xml_diff>
--- a/phaseshift/phaseshift_summary.xlsx
+++ b/phaseshift/phaseshift_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/phaseshift/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364270B0-7344-4247-BA0B-3075D1FFA41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8DE339-0664-A549-A35C-EC3DB0B9E2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phaseshift_metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>filename</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>2024-04-30_K_e.dat</t>
+  </si>
+  <si>
+    <t>2024-04-25_D_e.dat</t>
+  </si>
+  <si>
+    <t>2024-05-02_B_e.dat</t>
+  </si>
+  <si>
+    <t>2024-05-10_V_e.dat</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -939,13 +951,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1196,6 +1211,84 @@
         <v>20</v>
       </c>
       <c r="H9">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45407</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1.8</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>202.14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45414</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>1.8</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45422</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>1.8</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
         <v>202</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more phaseshift analysis and minor changes
</commit_message>
<xml_diff>
--- a/phaseshift/phaseshift_summary.xlsx
+++ b/phaseshift/phaseshift_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/phaseshift/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8DE339-0664-A549-A35C-EC3DB0B9E2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1D9C99-B8EF-FF4D-9201-3D996B82C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phaseshift_metadata" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>filename</t>
   </si>
@@ -110,6 +110,33 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>2024-06-10_R_e.dat</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>2024-06-12_W_e.dat</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>2024-06-13_I_e.dat</t>
+  </si>
+  <si>
+    <t>2024-06-13_L_e.dat</t>
+  </si>
+  <si>
+    <t>2024-06-14_D_e.dat</t>
+  </si>
+  <si>
+    <t>2024-06-17_I_e.dat</t>
+  </si>
+  <si>
+    <t>2024-06-18_D_e.dat</t>
   </si>
 </sst>
 </file>
@@ -951,15 +978,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1292,6 +1319,188 @@
         <v>202</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45453</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>1.8</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45455</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>1.8</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45456</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>1.8</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45456</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>1.8</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45457</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>1.8</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45460</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>1.8</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45461</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>1.8</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>